<commit_message>
updated eval_loop revisions_df outputs
</commit_message>
<xml_diff>
--- a/src/data/software_requirements_1.xlsx
+++ b/src/data/software_requirements_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/aiswre/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_0309E1E5B43B4C1E492C4CFF85290AE7787E8557" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA82A745-13E7-406B-A74A-B54658414B59}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_0309E1E5B43B4C1E492C4CFF85290AE7787E8557" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D96314CA-062A-4EF5-86A9-1F6438995E31}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Type</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>An error during this process means there was a problem parsing the sentence and creating the generic question. In this case, return a message such as Ã¢â‚¬Å“Sorry, I didnÃ¢â‚¬â„¢t understand that.Ã¢â‚¬Â</t>
+  </si>
+  <si>
+    <t>????erere ee</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,6 +474,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>